<commit_message>
update emmsap programs and files
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuthbert/git/emmsap/excelMetadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annagrau/Dropbox/EMMSAP/Anna_Cuthbert_PDFs/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="13240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
   <si>
     <t>2-3 motets</t>
-  </si>
-  <si>
-    <t>all</t>
   </si>
   <si>
     <t>2-3 mass/misc</t>
@@ -116,10 +113,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>#37 was missing; Wyatt fixing it</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>yes</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -185,50 +178,10 @@
     <t>(low priority -- mostly later music)</t>
   </si>
   <si>
-    <t>Scan and transribe #6 &amp; 30</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scan and transribe #77, 83, 84, 95</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Process</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>mostly</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Anna's notes</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Corwyn Wyatt</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Corwyn Wyatt</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jeremy Jennings</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assigned to Corwyn</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>need to process 30-49, Jeremy working on 49-84 now</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>If Jeremy finishes PMFC 11 I'll ask for help processing them-- he's been working more slowly since the baby</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Out to whom?</t>
   </si>
   <si>
@@ -251,33 +204,6 @@
   </si>
   <si>
     <t>1 Fauvel</t>
-  </si>
-  <si>
-    <t>mostly</t>
-  </si>
-  <si>
-    <t>Giovanni 8, 10-19</t>
-  </si>
-  <si>
-    <t>to 29</t>
-  </si>
-  <si>
-    <t>30-84</t>
-  </si>
-  <si>
-    <t>twa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14-16: Scanned by Solomon </t>
-  </si>
-  <si>
-    <t>Guhl-Muller for EMMSAP</t>
-  </si>
-  <si>
-    <t>but low priority</t>
-  </si>
-  <si>
-    <t>(not scanned)</t>
   </si>
   <si>
     <t>Marchi Turin</t>
@@ -299,18 +225,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Appendix f not done</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finish processing</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anna Grau</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>2-3 ballades</t>
   </si>
   <si>
@@ -323,21 +237,12 @@
     <t>E15cM 7</t>
   </si>
   <si>
-    <t>Jennings</t>
-  </si>
-  <si>
-    <t>first section</t>
-  </si>
-  <si>
     <t>(ot scanned) / Poznan 2 done</t>
   </si>
   <si>
     <t>Converted</t>
   </si>
   <si>
-    <t>done and awaiting processing.</t>
-  </si>
-  <si>
     <t>#11 Gloria Tenor is incomplete</t>
   </si>
   <si>
@@ -348,13 +253,62 @@
   </si>
   <si>
     <t>Finishing</t>
+  </si>
+  <si>
+    <t>(appendix e is incomplete but has a better version already in)</t>
+  </si>
+  <si>
+    <t>(some sections need converting)</t>
+  </si>
+  <si>
+    <t>OMR</t>
+  </si>
+  <si>
+    <t>Jeremy Jennings</t>
+  </si>
+  <si>
+    <t>14-16: Scanned by Solomon Guhl-Muller for EMMSAP</t>
+  </si>
+  <si>
+    <t>1-27 are done</t>
+  </si>
+  <si>
+    <t>"missing" pieces are in the Chantilly transcriptions</t>
+  </si>
+  <si>
+    <t>Old Hall MS</t>
+  </si>
+  <si>
+    <t>(This would be a big undertaking and require a lot more funding)</t>
+  </si>
+  <si>
+    <t>LONG FUTURE</t>
+  </si>
+  <si>
+    <t>Du Fay works</t>
+  </si>
+  <si>
+    <t>Las Huelgas Codex</t>
+  </si>
+  <si>
+    <t>Corwyn Wyatt</t>
+  </si>
+  <si>
+    <t>beginning with pieces ascribed to Vitry</t>
+  </si>
+  <si>
+    <t>through Stoessel and CMM files</t>
+  </si>
+  <si>
+    <t>motets, mass, hocket higher priority; lais lower</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +349,13 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -776,13 +737,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -796,492 +757,528 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>77</v>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="7"/>
       <c r="E31" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>92</v>
+        <v>54</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>99</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of recent changes....
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20260" windowHeight="15160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="91">
   <si>
     <t>2-3 motets</t>
   </si>
@@ -252,9 +252,6 @@
     <t>MSC</t>
   </si>
   <si>
-    <t>Finishing</t>
-  </si>
-  <si>
     <t>(appendix e is incomplete but has a better version already in)</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
   </si>
   <si>
     <t>Corwyn Wyatt</t>
-  </si>
-  <si>
-    <t>beginning with pieces ascribed to Vitry</t>
   </si>
   <si>
     <t>through Stoessel and CMM files</t>
@@ -302,6 +296,18 @@
   <si>
     <t>motets, mass, hocket higher priority; lais lower</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>finished pieces ascribe to Vitry</t>
+  </si>
+  <si>
+    <t>partly</t>
+  </si>
+  <si>
+    <t>process high priority, transcribe low priority</t>
   </si>
 </sst>
 </file>
@@ -743,7 +749,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -802,10 +808,13 @@
         <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -859,10 +868,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -950,7 +965,7 @@
         <v>54</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -997,7 +1012,7 @@
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -1010,10 +1025,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -1034,7 +1049,7 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -1049,7 +1064,7 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -1076,7 +1091,7 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -1195,13 +1210,16 @@
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1214,13 +1232,13 @@
         <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -1228,7 +1246,7 @@
         <v>44</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>42</v>
@@ -1255,30 +1273,30 @@
         <v>71</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add PMFC 22.47a (was missing)
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annagrau/Dropbox/EMMSAP/Anna_Cuthbert_PDFs/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuthbert/git/emmsap/excelMetadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20260" windowHeight="15160" tabRatio="500"/>
+    <workbookView xWindow="51820" yWindow="-10000" windowWidth="20260" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
   <si>
     <t>2-3 motets</t>
   </si>
@@ -109,10 +112,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>mostly</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>yes</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -150,10 +149,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Anna Grau</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>A lot of overlap with PMFC - so need to go carefully</t>
   </si>
   <si>
@@ -243,9 +238,6 @@
     <t>Converted</t>
   </si>
   <si>
-    <t>#11 Gloria Tenor is incomplete</t>
-  </si>
-  <si>
     <t>Prague 9</t>
   </si>
   <si>
@@ -289,9 +281,6 @@
   </si>
   <si>
     <t>Corwyn Wyatt</t>
-  </si>
-  <si>
-    <t>through Stoessel and CMM files</t>
   </si>
   <si>
     <t>motets, mass, hocket higher priority; lais lower</t>
@@ -308,13 +297,41 @@
   </si>
   <si>
     <t>process high priority, transcribe low priority</t>
+  </si>
+  <si>
+    <t>several pieces have no barlines; put barlines wherever convenient and to change time signatures as necessary.</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Myke Notes</t>
+  </si>
+  <si>
+    <t>done via Stoessel and CMM files</t>
+  </si>
+  <si>
+    <t>47a was skipped; added MSC</t>
+  </si>
+  <si>
+    <t>Josquin Research Project?</t>
+  </si>
+  <si>
+    <t>Other TODO:</t>
+  </si>
+  <si>
+    <t>Cowger often used slurs instead of ties -- these should be fixed algorithmically</t>
+  </si>
+  <si>
+    <t>(for Myke mostly)</t>
+  </si>
+  <si>
+    <t>Make sure that composers and titles are encoded properly in scores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -363,6 +380,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -388,7 +412,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -401,6 +425,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -743,13 +771,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -761,313 +789,318 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F24" s="3"/>
+      <c r="G24" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F25" s="3"/>
+      <c r="G25" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1075,11 +1108,11 @@
         <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1087,75 +1120,76 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="7"/>
       <c r="E31" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -1163,7 +1197,7 @@
         <v>24</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -1171,132 +1205,151 @@
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many new OMR files
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuthbert/git/emmsap/excelMetadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annagrau/Dropbox/EMMSAP/Anna_Cuthbert_PDFs/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51820" yWindow="-10000" windowWidth="20260" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="20260" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
   <si>
     <t>2-3 motets</t>
   </si>
@@ -207,12 +207,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>12-14 -- see the CPDL folder in the EMMSAP folder -- need to be converted and then included</t>
-  </si>
-  <si>
     <t>new discoveries</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>E15cM 7</t>
   </si>
   <si>
-    <t>(ot scanned) / Poznan 2 done</t>
-  </si>
-  <si>
     <t>Converted</t>
   </si>
   <si>
@@ -257,9 +248,6 @@
   </si>
   <si>
     <t>14-16: Scanned by Solomon Guhl-Muller for EMMSAP</t>
-  </si>
-  <si>
-    <t>1-27 are done</t>
   </si>
   <si>
     <t>"missing" pieces are in the Chantilly transcriptions</t>
@@ -325,6 +313,24 @@
   </si>
   <si>
     <t>Make sure that composers and titles are encoded properly in scores</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>All but one piece by N. Zacharie and all of Antonius Romanus are done</t>
+  </si>
+  <si>
+    <t>Myke working on it -- all of Poznan and Warsaw done; leaving 1/2 of Kras.</t>
+  </si>
+  <si>
+    <t>14-15 not too important so MSC did it as OMR (fast but</t>
+  </si>
+  <si>
+    <t>inaccurate);  This will be good enough for now.</t>
   </si>
 </sst>
 </file>
@@ -774,10 +780,10 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -809,7 +815,7 @@
         <v>46</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -839,18 +845,18 @@
         <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>52</v>
@@ -862,7 +868,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -874,7 +880,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -899,16 +905,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -963,10 +969,10 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -996,7 +1002,7 @@
         <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -1039,27 +1045,45 @@
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>72</v>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1081,7 +1105,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1097,7 +1121,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -1124,7 +1148,7 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1139,7 +1163,7 @@
       </c>
       <c r="E28" s="3"/>
       <c r="G28" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
@@ -1167,9 +1191,6 @@
       <c r="B30" s="3"/>
       <c r="D30" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1189,42 +1210,45 @@
         <v>56</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1256,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>31</v>
       </c>
@@ -1240,58 +1264,67 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="D43" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
@@ -1299,57 +1332,57 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of new data...
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annagrau/Dropbox/EMMSAP/Anna_Cuthbert_PDFs/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuthbert/git/emmsap/excelMetadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="20260" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="7060" yWindow="1420" windowWidth="20260" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>2-3 motets</t>
   </si>
@@ -149,12 +149,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>A lot of overlap with PMFC - so need to go carefully</t>
-  </si>
-  <si>
-    <t>Early 15th C. Music</t>
-  </si>
-  <si>
     <t>(owned as loose leaf by MSC)</t>
   </si>
   <si>
@@ -271,26 +265,19 @@
     <t>Corwyn Wyatt</t>
   </si>
   <si>
-    <t>motets, mass, hocket higher priority; lais lower</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>finished pieces ascribe to Vitry</t>
+  </si>
+  <si>
+    <t>partly</t>
+  </si>
+  <si>
+    <t>several pieces have no barlines; put barlines wherever convenient and to change time signatures as necessary.</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>finished pieces ascribe to Vitry</t>
-  </si>
-  <si>
-    <t>partly</t>
-  </si>
-  <si>
-    <t>process high priority, transcribe low priority</t>
-  </si>
-  <si>
-    <t>several pieces have no barlines; put barlines wherever convenient and to change time signatures as necessary.</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>Myke Notes</t>
   </si>
   <si>
@@ -306,9 +293,6 @@
     <t>Other TODO:</t>
   </si>
   <si>
-    <t>Cowger often used slurs instead of ties -- these should be fixed algorithmically</t>
-  </si>
-  <si>
     <t>(for Myke mostly)</t>
   </si>
   <si>
@@ -331,13 +315,25 @@
   </si>
   <si>
     <t>inaccurate);  This will be good enough for now.</t>
+  </si>
+  <si>
+    <t>Kelsey Cowger often used slurs instead of ties -- these should be fixed algorithmically</t>
+  </si>
+  <si>
+    <t>2 lais</t>
+  </si>
+  <si>
+    <t>yes/OMR</t>
+  </si>
+  <si>
+    <t>Antonius de Cividale by Hand (Jennings), rest OMR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -378,13 +374,6 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -777,13 +766,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -800,93 +789,93 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -894,495 +883,519 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>4</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="8" t="s">
-        <v>85</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="G28" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="G29" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="D30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
-      <c r="E31" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>52</v>
+      <c r="B31" s="3"/>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="7"/>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>94</v>
+        <v>32</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>89</v>
+        <v>73</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all this XML data!
</commit_message>
<xml_diff>
--- a/excelMetadata/project_overview.xlsx
+++ b/excelMetadata/project_overview.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuthbert/git/emmsap/excelMetadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annagrau/Dropbox/EMMSAP/Anna_Cuthbert_PDFs/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="1420" windowWidth="20260" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="5340" yWindow="1420" windowWidth="20260" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="96">
   <si>
     <t>2-3 motets</t>
   </si>
@@ -293,15 +293,6 @@
     <t>Make sure that composers and titles are encoded properly in scores</t>
   </si>
   <si>
-    <t>processing</t>
-  </si>
-  <si>
-    <t>process</t>
-  </si>
-  <si>
-    <t>All but one piece by N. Zacharie and all of Antonius Romanus are done</t>
-  </si>
-  <si>
     <t>14-15 not too important so MSC did it as OMR (fast but</t>
   </si>
   <si>
@@ -330,6 +321,9 @@
   </si>
   <si>
     <t>Myke working on it -- all of Poznan and Warsaw done;  1/2 of Kras. done as OMR</t>
+  </si>
+  <si>
+    <t>McGee</t>
   </si>
 </sst>
 </file>
@@ -769,13 +763,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -894,7 +888,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>64</v>
@@ -1050,7 +1044,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>66</v>
@@ -1067,7 +1061,7 @@
         <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1077,8 +1071,8 @@
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>86</v>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F23" t="s">
         <v>77</v>
@@ -1244,10 +1238,10 @@
         <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
@@ -1287,8 +1281,8 @@
       <c r="C40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>85</v>
+      <c r="D40" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
@@ -1296,13 +1290,13 @@
         <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -1312,8 +1306,11 @@
       <c r="B42" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>87</v>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
@@ -1349,12 +1346,12 @@
         <v>41</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>64</v>
@@ -1365,10 +1362,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
@@ -1382,45 +1379,56 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="4" t="s">
-        <v>70</v>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="4" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B58" s="8" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>